<commit_message>
Added state tables and transition functions for addition, subtraction, and multiplication.
</commit_message>
<xml_diff>
--- a/Project_1/State_Table.xlsx
+++ b/Project_1/State_Table.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\algorithms\Project_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rogerjm1\Documents\Gitlab\algorithms\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2FC22CF-CFC7-46D5-A2C8-0AA71A3DD888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30975" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{F64A7F81-ABF4-432F-B904-9F8DD77F99EB}"/>
+    <workbookView xWindow="30972" yWindow="2208" windowWidth="21600" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="64">
   <si>
     <t>Q - {qY, qN}</t>
   </si>
@@ -148,12 +147,87 @@
   </si>
   <si>
     <t>Addition Table</t>
+  </si>
+  <si>
+    <t>Subtraction Table</t>
+  </si>
+  <si>
+    <t>q3, b, -1</t>
+  </si>
+  <si>
+    <t>q4, b, -1</t>
+  </si>
+  <si>
+    <t>q9, x, 1</t>
+  </si>
+  <si>
+    <t>q5, x, -1</t>
+  </si>
+  <si>
+    <t>q5, 1, -1</t>
+  </si>
+  <si>
+    <t>q6,x,-1</t>
+  </si>
+  <si>
+    <t>q6, 1, -1</t>
+  </si>
+  <si>
+    <t>q7, x, 1</t>
+  </si>
+  <si>
+    <t>Multiplication Table</t>
+  </si>
+  <si>
+    <t>q9, b, 1</t>
+  </si>
+  <si>
+    <t>qY, b, 0</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>qN, j, 0</t>
+  </si>
+  <si>
+    <t>q3, j, 1</t>
+  </si>
+  <si>
+    <t>multiply by 0</t>
+  </si>
+  <si>
+    <t>q8, 1, -1</t>
+  </si>
+  <si>
+    <t>qN, 1, 0</t>
+  </si>
+  <si>
+    <t>q7, 1, -1</t>
+  </si>
+  <si>
+    <t>qY, x, 0</t>
+  </si>
+  <si>
+    <t>q2, b, 1</t>
+  </si>
+  <si>
+    <t>q3, x, 1</t>
+  </si>
+  <si>
+    <t>q4, j, 1</t>
+  </si>
+  <si>
+    <t>q4, 1, 1</t>
+  </si>
+  <si>
+    <t>q8, x, -1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +290,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,26 +608,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BA5A8E-DA6B-477C-8F3B-FE2A1E8511DC}">
-  <dimension ref="C3:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -596,7 +674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -619,7 +697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
@@ -642,7 +720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,7 +743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
@@ -688,7 +766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -711,7 +789,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -734,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -757,7 +835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
@@ -780,7 +858,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
@@ -803,117 +881,447 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="1" t="s">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="3" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="3">
+      <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="3" t="s">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G21" s="3" t="s">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="3" t="s">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="3" t="s">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="3" t="s">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="E24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="E30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="3" t="s">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="F36" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>